<commit_message>
Se agregan endpoints y validaciones
</commit_message>
<xml_diff>
--- a/excelReports/InterferReport.xlsx
+++ b/excelReports/InterferReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Company</t>
   </si>
@@ -86,6 +86,30 @@
   </si>
   <si>
     <t>CCC</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>ZZZZZZZZZZ</t>
+  </si>
+  <si>
+    <t>AAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>XCVSAMDVSDJKLANFKLJASDNFLJKSNADL</t>
+  </si>
+  <si>
+    <t>XCVSAMDVSDJKLANFK</t>
   </si>
 </sst>
 </file>
@@ -132,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="1" applyFill="1" fillId="2"/>
+    <xf applyFont="1" fontId="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,7 +169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -175,7 +200,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -192,7 +217,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -209,7 +234,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -226,7 +251,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -243,7 +268,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -260,7 +285,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -277,7 +302,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -294,7 +319,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -311,7 +336,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -328,7 +353,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -345,7 +370,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -362,7 +387,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -379,7 +404,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -396,7 +421,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -413,7 +438,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -430,7 +455,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -447,7 +472,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -461,6 +486,108 @@
       </c>
       <c r="E18" s="0" t="n">
         <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>